<commit_message>
Women LEd changes on OppDetailpage 10/17/2025
</commit_message>
<xml_diff>
--- a/TestData/LV_1_CF_TMTT0049771_VerifyMergersAcquisitionsMAChangesInOpportunityCreationToEngagementConversionWithTheApprovalProcess.xlsx
+++ b/TestData/LV_1_CF_TMTT0049771_VerifyMergersAcquisitionsMAChangesInOpportunityCreationToEngagementConversionWithTheApprovalProcess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9769747-10BE-41B6-B9EC-5429D6459AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC9D490-13A5-426A-8849-5998347985E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="548" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StandardUsers" sheetId="2" r:id="rId1"/>
@@ -1124,14 +1124,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1142,7 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1176,13 +1177,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBB8EB1-471A-4668-845A-6810E22F6BA4}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>

</xml_diff>